<commit_message>
Updated Visualisation and renaming and reordering scripts
</commit_message>
<xml_diff>
--- a/Data/02_Homologs_precalculated/Homologs_Renamed_Seqkit.xlsx
+++ b/Data/02_Homologs_precalculated/Homologs_Renamed_Seqkit.xlsx
@@ -8482,9 +8482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCA6D8C-85DC-4746-9FBE-17B8FEED5CFD}">
   <dimension ref="A1:D939"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -22580,7 +22578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A029087-DA3A-5F47-8FB7-4A71C07B18C2}">
   <dimension ref="A1:G938"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>